<commit_message>
17 фев 2023 г. 15:32:40
</commit_message>
<xml_diff>
--- a/fh/lab1/Lab1_solution/main.xlsx
+++ b/fh/lab1/Lab1_solution/main.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\4sem\fh\lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\4sem\fh\lab1\Lab1_solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58271D9F-B401-4B8F-A7CB-EFDAFCCF9E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21ACD9B-2FE7-48A8-B53E-6D9AF8AA0C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,164 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
-  <si>
-    <t>-133820.765566</t>
-  </si>
-  <si>
-    <t>-133664.678776</t>
-  </si>
-  <si>
-    <t>-133505.607238</t>
-  </si>
-  <si>
-    <t>-133343.550179</t>
-  </si>
-  <si>
-    <t>-133178.507793</t>
-  </si>
-  <si>
-    <t>-133010.481242</t>
-  </si>
-  <si>
-    <t>-132839.472660</t>
-  </si>
-  <si>
-    <t>-132665.485154</t>
-  </si>
-  <si>
-    <t>-132488.522806</t>
-  </si>
-  <si>
-    <t>-132308.590678</t>
-  </si>
-  <si>
-    <t>-132125.694811</t>
-  </si>
-  <si>
-    <t>-131939.842231</t>
-  </si>
-  <si>
-    <t>-131751.040946</t>
-  </si>
-  <si>
-    <t>-131559.299956</t>
-  </si>
-  <si>
-    <t>-131364.629248</t>
-  </si>
-  <si>
-    <t>-131167.039803</t>
-  </si>
-  <si>
-    <t>-130966.543598</t>
-  </si>
-  <si>
-    <t>-130763.153603</t>
-  </si>
-  <si>
-    <t>-130556.883794</t>
-  </si>
-  <si>
-    <t>-130347.749145</t>
-  </si>
-  <si>
-    <t>-130135.765634</t>
-  </si>
-  <si>
-    <t>-129920.950250</t>
-  </si>
-  <si>
-    <t>-129703.320987</t>
-  </si>
-  <si>
-    <t>-129482.896854</t>
-  </si>
-  <si>
-    <t>-129259.697871</t>
-  </si>
-  <si>
-    <t>-129033.745077</t>
-  </si>
-  <si>
-    <t>-128805.060530</t>
-  </si>
-  <si>
-    <t>-128573.667306</t>
-  </si>
-  <si>
-    <t>-128339.589509</t>
-  </si>
-  <si>
-    <t>-128102.852267</t>
-  </si>
-  <si>
-    <t>-127863.481736</t>
-  </si>
-  <si>
-    <t>-127621.505103</t>
-  </si>
-  <si>
-    <t>-127376.950589</t>
-  </si>
-  <si>
-    <t>-127129.847450</t>
-  </si>
-  <si>
-    <t>-126880.225981</t>
-  </si>
-  <si>
-    <t>-126628.117516</t>
-  </si>
-  <si>
-    <t>-126373.554432</t>
-  </si>
-  <si>
-    <t>-126116.570154</t>
-  </si>
-  <si>
-    <t>-125857.199149</t>
-  </si>
-  <si>
-    <t>-125595.476940</t>
-  </si>
-  <si>
-    <t>-125331.440099</t>
-  </si>
-  <si>
-    <t>-125065.126252</t>
-  </si>
-  <si>
-    <t>-124796.574085</t>
-  </si>
-  <si>
-    <t>-124525.823341</t>
-  </si>
-  <si>
-    <t>-124252.914827</t>
-  </si>
-  <si>
-    <t>-123977.890412</t>
-  </si>
-  <si>
-    <t>-123700.793035</t>
-  </si>
-  <si>
-    <t>-123421.666701</t>
-  </si>
-  <si>
-    <t>-123140.556487</t>
-  </si>
-  <si>
-    <t>-122857.508546</t>
-  </si>
-  <si>
-    <t>-122572.570105</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -213,8 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -325,7 +170,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$3</c:f>
+              <c:f>Лист1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -344,167 +189,6 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Лист1!$C$4:$C$54</c:f>
-              <c:strCache>
-                <c:ptCount val="51"/>
-                <c:pt idx="0">
-                  <c:v>-133820.765566</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-133664.678776</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-133505.607238</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-133343.550179</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-133178.507793</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-133010.481242</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-132839.472660</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-132665.485154</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-132488.522806</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-132308.590678</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-132125.694811</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-131939.842231</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-131751.040946</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-131559.299956</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-131364.629248</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-131167.039803</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-130966.543598</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-130763.153603</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-130556.883794</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-130347.749145</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-130135.765634</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-129920.950250</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-129703.320987</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-129482.896854</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-129259.697871</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-129033.745077</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-128805.060530</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-128573.667306</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-128339.589509</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-128102.852267</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-127863.481736</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-127621.505103</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-127376.950589</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-127129.847450</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-126880.225981</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-126628.117516</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-126373.554432</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-126116.570154</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-125857.199149</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>-125595.476940</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>-125331.440099</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>-125065.126252</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>-124796.574085</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>-124525.823341</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>-124252.914827</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>-123977.890412</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>-123700.793035</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>-123421.666701</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-123140.556487</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>-122857.508546</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-122572.570105</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
               <c:f>Лист1!$B$4:$B$54</c:f>
               <c:numCache>
@@ -662,6 +346,168 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$4:$C$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>-133820.76556599999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-133664.67877599999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-133505.607238</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-133343.55017900001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-133178.507793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-133010.48124200001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-132839.47266</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-132665.48515399999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-132488.52280599999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-132308.59067800001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-132125.69481099999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-131939.84223099999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-131751.04094599999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-131559.299956</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-131364.62924800001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-131167.03980299999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-130966.543598</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-130763.153603</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-130556.88379399999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-130347.74914499999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-130135.765634</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-129920.95024999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-129703.320987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-129482.89685400001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-129259.697871</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-129033.745077</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-128805.06053</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-128573.667306</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-128339.589509</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-128102.85226699999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-127863.481736</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-127621.505103</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-127376.950589</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-127129.84745</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-126880.225981</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-126628.117516</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-126373.554432</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-126116.570154</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-125857.19914899999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-125595.47693999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-125331.440099</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-125065.126252</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-124796.574085</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-124525.823341</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-124252.914827</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-123977.89041199999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-123700.793035</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-123421.66670099999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-123140.55648699999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-122857.508546</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-122572.57010500001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -713,11 +559,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>Тепловой</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="ru-RU" baseline="0"/>
-                  <a:t> эффект реакции</a:t>
+                  <a:t>Температура</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -753,9 +595,9 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -838,7 +680,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>Температура</a:t>
+                  <a:t>Тепловой эффект</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1519,16 +1361,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>40251</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>81510</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2728793</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>164933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>255195</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>120138</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>61248</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>15948</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1819,10 +1661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:C54"/>
+  <dimension ref="B3:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="62" workbookViewId="0">
-      <selection activeCell="X29" sqref="X29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="66" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,413 +1672,419 @@
     <col min="3" max="3" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+    </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="1">
         <v>500</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
+      <c r="C4" s="1">
+        <v>-133820.76556599999</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="1">
         <v>510</v>
       </c>
-      <c r="C5" t="s">
-        <v>1</v>
+      <c r="C5" s="1">
+        <v>-133664.67877599999</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="1">
         <v>520</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
+      <c r="C6" s="1">
+        <v>-133505.607238</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="B7" s="1">
         <v>530</v>
       </c>
-      <c r="C7" t="s">
-        <v>3</v>
+      <c r="C7" s="1">
+        <v>-133343.55017900001</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="1">
         <v>540</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
+      <c r="C8" s="1">
+        <v>-133178.507793</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="B9" s="1">
         <v>550</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
+      <c r="C9" s="1">
+        <v>-133010.48124200001</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="1">
         <v>560</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
+      <c r="C10" s="1">
+        <v>-132839.47266</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="1">
         <v>570</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
+      <c r="C11" s="1">
+        <v>-132665.48515399999</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="1">
         <v>580</v>
       </c>
-      <c r="C12" t="s">
-        <v>8</v>
+      <c r="C12" s="1">
+        <v>-132488.52280599999</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="B13" s="1">
         <v>590</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
+      <c r="C13" s="1">
+        <v>-132308.59067800001</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="1">
         <v>600</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
+      <c r="C14" s="1">
+        <v>-132125.69481099999</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="1">
         <v>610</v>
       </c>
-      <c r="C15" t="s">
-        <v>11</v>
+      <c r="C15" s="1">
+        <v>-131939.84223099999</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B16" s="1">
         <v>620</v>
       </c>
-      <c r="C16" t="s">
-        <v>12</v>
+      <c r="C16" s="1">
+        <v>-131751.04094599999</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="B17" s="1">
         <v>630</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
+      <c r="C17" s="1">
+        <v>-131559.299956</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="B18" s="1">
         <v>640</v>
       </c>
-      <c r="C18" t="s">
-        <v>14</v>
+      <c r="C18" s="1">
+        <v>-131364.62924800001</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="B19" s="1">
         <v>650</v>
       </c>
-      <c r="C19" t="s">
-        <v>15</v>
+      <c r="C19" s="1">
+        <v>-131167.03980299999</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="B20" s="1">
         <v>660</v>
       </c>
-      <c r="C20" t="s">
-        <v>16</v>
+      <c r="C20" s="1">
+        <v>-130966.543598</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="B21" s="1">
         <v>670</v>
       </c>
-      <c r="C21" t="s">
-        <v>17</v>
+      <c r="C21" s="1">
+        <v>-130763.153603</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="B22" s="1">
         <v>680</v>
       </c>
-      <c r="C22" t="s">
-        <v>18</v>
+      <c r="C22" s="1">
+        <v>-130556.88379399999</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="B23" s="1">
         <v>690</v>
       </c>
-      <c r="C23" t="s">
-        <v>19</v>
+      <c r="C23" s="1">
+        <v>-130347.74914499999</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="B24" s="1">
         <v>700</v>
       </c>
-      <c r="C24" t="s">
-        <v>20</v>
+      <c r="C24" s="1">
+        <v>-130135.765634</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="B25" s="1">
         <v>710</v>
       </c>
-      <c r="C25" t="s">
-        <v>21</v>
+      <c r="C25" s="1">
+        <v>-129920.95024999999</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="B26" s="1">
         <v>720</v>
       </c>
-      <c r="C26" t="s">
-        <v>22</v>
+      <c r="C26" s="1">
+        <v>-129703.320987</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="B27" s="1">
         <v>730</v>
       </c>
-      <c r="C27" t="s">
-        <v>23</v>
+      <c r="C27" s="1">
+        <v>-129482.89685400001</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="B28" s="1">
         <v>740</v>
       </c>
-      <c r="C28" t="s">
-        <v>24</v>
+      <c r="C28" s="1">
+        <v>-129259.697871</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29">
+      <c r="B29" s="1">
         <v>750</v>
       </c>
-      <c r="C29" t="s">
-        <v>25</v>
+      <c r="C29" s="1">
+        <v>-129033.745077</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30">
+      <c r="B30" s="1">
         <v>760</v>
       </c>
-      <c r="C30" t="s">
-        <v>26</v>
+      <c r="C30" s="1">
+        <v>-128805.06053</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31">
+      <c r="B31" s="1">
         <v>770</v>
       </c>
-      <c r="C31" t="s">
-        <v>27</v>
+      <c r="C31" s="1">
+        <v>-128573.667306</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32">
+      <c r="B32" s="1">
         <v>780</v>
       </c>
-      <c r="C32" t="s">
-        <v>28</v>
+      <c r="C32" s="1">
+        <v>-128339.589509</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33">
+      <c r="B33" s="1">
         <v>790</v>
       </c>
-      <c r="C33" t="s">
-        <v>29</v>
+      <c r="C33" s="1">
+        <v>-128102.85226699999</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34">
+      <c r="B34" s="1">
         <v>800</v>
       </c>
-      <c r="C34" t="s">
-        <v>30</v>
+      <c r="C34" s="1">
+        <v>-127863.481736</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35">
+      <c r="B35" s="1">
         <v>810</v>
       </c>
-      <c r="C35" t="s">
-        <v>31</v>
+      <c r="C35" s="1">
+        <v>-127621.505103</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36">
+      <c r="B36" s="1">
         <v>820</v>
       </c>
-      <c r="C36" t="s">
-        <v>32</v>
+      <c r="C36" s="1">
+        <v>-127376.950589</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37">
+      <c r="B37" s="1">
         <v>830</v>
       </c>
-      <c r="C37" t="s">
-        <v>33</v>
+      <c r="C37" s="1">
+        <v>-127129.84745</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38">
+      <c r="B38" s="1">
         <v>840</v>
       </c>
-      <c r="C38" t="s">
-        <v>34</v>
+      <c r="C38" s="1">
+        <v>-126880.225981</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39">
+      <c r="B39" s="1">
         <v>850</v>
       </c>
-      <c r="C39" t="s">
-        <v>35</v>
+      <c r="C39" s="1">
+        <v>-126628.117516</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40">
+      <c r="B40" s="1">
         <v>860</v>
       </c>
-      <c r="C40" t="s">
-        <v>36</v>
+      <c r="C40" s="1">
+        <v>-126373.554432</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41">
+      <c r="B41" s="1">
         <v>870</v>
       </c>
-      <c r="C41" t="s">
-        <v>37</v>
+      <c r="C41" s="1">
+        <v>-126116.570154</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42">
+      <c r="B42" s="1">
         <v>880</v>
       </c>
-      <c r="C42" t="s">
-        <v>38</v>
+      <c r="C42" s="1">
+        <v>-125857.19914899999</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43">
+      <c r="B43" s="1">
         <v>890</v>
       </c>
-      <c r="C43" t="s">
-        <v>39</v>
+      <c r="C43" s="1">
+        <v>-125595.47693999999</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44">
+      <c r="B44" s="1">
         <v>900</v>
       </c>
-      <c r="C44" t="s">
-        <v>40</v>
+      <c r="C44" s="1">
+        <v>-125331.440099</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45">
+      <c r="B45" s="1">
         <v>910</v>
       </c>
-      <c r="C45" t="s">
-        <v>41</v>
+      <c r="C45" s="1">
+        <v>-125065.126252</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46">
+      <c r="B46" s="1">
         <v>920</v>
       </c>
-      <c r="C46" t="s">
-        <v>42</v>
+      <c r="C46" s="1">
+        <v>-124796.574085</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47">
+      <c r="B47" s="1">
         <v>930</v>
       </c>
-      <c r="C47" t="s">
-        <v>43</v>
+      <c r="C47" s="1">
+        <v>-124525.823341</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48">
+      <c r="B48" s="1">
         <v>940</v>
       </c>
-      <c r="C48" t="s">
-        <v>44</v>
+      <c r="C48" s="1">
+        <v>-124252.914827</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49">
+      <c r="B49" s="1">
         <v>950</v>
       </c>
-      <c r="C49" t="s">
-        <v>45</v>
+      <c r="C49" s="1">
+        <v>-123977.89041199999</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50">
+      <c r="B50" s="1">
         <v>960</v>
       </c>
-      <c r="C50" t="s">
-        <v>46</v>
+      <c r="C50" s="1">
+        <v>-123700.793035</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51">
+      <c r="B51" s="1">
         <v>970</v>
       </c>
-      <c r="C51" t="s">
-        <v>47</v>
+      <c r="C51" s="1">
+        <v>-123421.66670099999</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52">
+      <c r="B52" s="1">
         <v>980</v>
       </c>
-      <c r="C52" t="s">
-        <v>48</v>
+      <c r="C52" s="1">
+        <v>-123140.55648699999</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53">
+      <c r="B53" s="1">
         <v>990</v>
       </c>
-      <c r="C53" t="s">
-        <v>49</v>
+      <c r="C53" s="1">
+        <v>-122857.508546</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54">
+      <c r="B54" s="1">
         <v>1000</v>
       </c>
-      <c r="C54" t="s">
-        <v>50</v>
-      </c>
+      <c r="C54" s="1">
+        <v>-122572.57010500001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>